<commit_message>
feat: add production report generation script and update template
refactor(production_followup2.py): switch from HTML parsing to CSV input
feat: add pandas dependency for CSV processing
docs: update unit names and data mapping in template
test: add test.ipynb for data processing validation
</commit_message>
<xml_diff>
--- a/01. Jan/31.xlsx
+++ b/01. Jan/31.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\1. Daily\Production follow up\01. Jan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. Work\1. Daily\Production follow up\01. Jan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BE5F08-874B-42AE-BFAE-F9BD648A2317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EC6460-DA0C-48E8-8F90-FB53E356E7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t xml:space="preserve">Date: </t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Plan vs Achievement</t>
   </si>
 </sst>
 </file>
@@ -200,23 +203,27 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -596,11 +603,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X21"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R11" sqref="R11:S11"/>
+      <selection pane="topRight" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,225 +618,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
         <f ca="1">TODAY() - 1</f>
-        <v>45690</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+        <v>46013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="5">
-        <v>86329</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2656739.333333333</v>
-      </c>
-      <c r="D3" s="5">
-        <v>2681465</v>
-      </c>
-      <c r="E3" s="4">
-        <v>-24725.666666666511</v>
-      </c>
-      <c r="F3" s="5">
-        <v>2656739</v>
-      </c>
-      <c r="G3" s="4">
-        <v>-24726</v>
-      </c>
-      <c r="H3" s="5">
-        <v>61603</v>
-      </c>
-      <c r="I3" s="5">
-        <v>406579</v>
-      </c>
-      <c r="J3" s="5">
-        <v>579267</v>
-      </c>
-      <c r="K3" s="5">
-        <v>91202</v>
-      </c>
-      <c r="L3" s="10">
-        <v>1.0261</v>
-      </c>
-      <c r="M3" s="5">
-        <v>6160</v>
-      </c>
-      <c r="N3" s="4">
-        <v>6.6</v>
-      </c>
-      <c r="O3" s="4">
-        <v>6.71</v>
-      </c>
-      <c r="P3" s="4">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>11.07</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" s="5">
-        <v>17992630</v>
-      </c>
-      <c r="U3" s="5">
-        <v>17534477</v>
-      </c>
-      <c r="V3" s="4">
-        <v>27</v>
-      </c>
-      <c r="W3" s="4">
-        <v>27</v>
-      </c>
-      <c r="X3" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5">
-        <v>8860</v>
+        <v>86329</v>
       </c>
       <c r="C4" s="5">
-        <v>302835.66666666669</v>
+        <v>2656739.333333333</v>
       </c>
       <c r="D4" s="5">
-        <v>295870</v>
-      </c>
-      <c r="E4" s="5">
-        <v>6965.6666666666861</v>
+        <v>2681465</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-24725.666666666511</v>
       </c>
       <c r="F4" s="5">
-        <v>302835</v>
-      </c>
-      <c r="G4" s="5">
-        <v>6965</v>
+        <v>2656739</v>
+      </c>
+      <c r="G4" s="4">
+        <v>-24726</v>
       </c>
       <c r="H4" s="5">
-        <v>15825</v>
+        <v>61603</v>
       </c>
       <c r="I4" s="5">
-        <v>85613</v>
+        <v>406579</v>
       </c>
       <c r="J4" s="5">
-        <v>45983</v>
+        <v>579267</v>
       </c>
       <c r="K4" s="5">
-        <v>9748</v>
+        <v>91202</v>
       </c>
       <c r="L4" s="10">
-        <v>0.93720000000000003</v>
+        <v>1.0261</v>
       </c>
       <c r="M4" s="5">
-        <v>1582</v>
+        <v>6160</v>
       </c>
       <c r="N4" s="4">
-        <v>5.41</v>
+        <v>6.6</v>
       </c>
       <c r="O4" s="4">
-        <v>5.19</v>
+        <v>6.71</v>
       </c>
       <c r="P4" s="4">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
-        <v>10.66</v>
+        <v>11.07</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="T4" s="5">
-        <v>1535565</v>
+        <v>17992630</v>
       </c>
       <c r="U4" s="5">
-        <v>1638337</v>
+        <v>17534477</v>
       </c>
       <c r="V4" s="4">
         <v>27</v>
@@ -843,67 +781,67 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5">
-        <v>67094</v>
+        <v>8860</v>
       </c>
       <c r="C5" s="5">
-        <v>1592305</v>
+        <v>302835.66666666669</v>
       </c>
       <c r="D5" s="5">
-        <v>1551739</v>
+        <v>295870</v>
       </c>
       <c r="E5" s="5">
-        <v>40566</v>
+        <v>6965.6666666666861</v>
       </c>
       <c r="F5" s="5">
-        <v>1592305</v>
+        <v>302835</v>
       </c>
       <c r="G5" s="5">
-        <v>40566</v>
+        <v>6965</v>
       </c>
       <c r="H5" s="5">
-        <v>107660</v>
+        <v>15825</v>
       </c>
       <c r="I5" s="5">
-        <v>701943</v>
+        <v>85613</v>
       </c>
       <c r="J5" s="5">
-        <v>438794</v>
+        <v>45983</v>
       </c>
       <c r="K5" s="5">
-        <v>61518</v>
+        <v>9748</v>
       </c>
       <c r="L5" s="10">
-        <v>0.97750000000000004</v>
+        <v>0.93720000000000003</v>
       </c>
       <c r="M5" s="5">
-        <v>9787</v>
+        <v>1582</v>
       </c>
       <c r="N5" s="4">
-        <v>6.52</v>
+        <v>5.41</v>
       </c>
       <c r="O5" s="4">
-        <v>6.54</v>
+        <v>5.19</v>
       </c>
       <c r="P5" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="4">
-        <v>12.24</v>
+        <v>10.66</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="T5" s="5">
-        <v>10148373</v>
+        <v>1535565</v>
       </c>
       <c r="U5" s="5">
-        <v>10381828</v>
+        <v>1638337</v>
       </c>
       <c r="V5" s="4">
         <v>27</v>
@@ -917,67 +855,67 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5">
-        <v>75111</v>
+        <v>67094</v>
       </c>
       <c r="C6" s="5">
-        <v>2153057</v>
+        <v>1592305</v>
       </c>
       <c r="D6" s="5">
-        <v>2223031</v>
-      </c>
-      <c r="E6" s="4">
-        <v>-69974</v>
+        <v>1551739</v>
+      </c>
+      <c r="E6" s="5">
+        <v>40566</v>
       </c>
       <c r="F6" s="5">
-        <v>2153057</v>
-      </c>
-      <c r="G6" s="4">
-        <v>-69974</v>
+        <v>1592305</v>
+      </c>
+      <c r="G6" s="5">
+        <v>40566</v>
       </c>
       <c r="H6" s="5">
-        <v>5137</v>
+        <v>107660</v>
       </c>
       <c r="I6" s="5">
-        <v>48904</v>
+        <v>701943</v>
       </c>
       <c r="J6" s="5">
-        <v>666985</v>
+        <v>438794</v>
       </c>
       <c r="K6" s="5">
-        <v>90069</v>
+        <v>61518</v>
       </c>
       <c r="L6" s="10">
-        <v>0.96299999999999997</v>
-      </c>
-      <c r="M6" s="4">
-        <v>570</v>
+        <v>0.97750000000000004</v>
+      </c>
+      <c r="M6" s="5">
+        <v>9787</v>
       </c>
       <c r="N6" s="4">
-        <v>9.52</v>
+        <v>6.52</v>
       </c>
       <c r="O6" s="4">
-        <v>8.8800000000000008</v>
+        <v>6.54</v>
       </c>
       <c r="P6" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="Q6" s="4">
-        <v>11.1</v>
-      </c>
-      <c r="R6" s="10">
-        <v>0.67</v>
-      </c>
-      <c r="S6" s="10">
-        <v>0.61699999999999999</v>
+        <v>12.24</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="T6" s="5">
-        <v>19740515</v>
+        <v>10148373</v>
       </c>
       <c r="U6" s="5">
-        <v>20497102</v>
+        <v>10381828</v>
       </c>
       <c r="V6" s="4">
         <v>27</v>
@@ -991,67 +929,67 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="5">
-        <v>62425</v>
+        <v>75111</v>
       </c>
       <c r="C7" s="5">
-        <v>2222421</v>
+        <v>2153057</v>
       </c>
       <c r="D7" s="5">
-        <v>2213551</v>
-      </c>
-      <c r="E7" s="5">
-        <v>8870</v>
+        <v>2223031</v>
+      </c>
+      <c r="E7" s="4">
+        <v>-69974</v>
       </c>
       <c r="F7" s="5">
-        <v>2222421</v>
-      </c>
-      <c r="G7" s="5">
-        <v>8870</v>
+        <v>2153057</v>
+      </c>
+      <c r="G7" s="4">
+        <v>-69974</v>
       </c>
       <c r="H7" s="5">
-        <v>71295</v>
+        <v>5137</v>
       </c>
       <c r="I7" s="5">
-        <v>492648</v>
+        <v>48904</v>
       </c>
       <c r="J7" s="5">
-        <v>425114</v>
+        <v>666985</v>
       </c>
       <c r="K7" s="5">
-        <v>71526</v>
+        <v>90069</v>
       </c>
       <c r="L7" s="10">
-        <v>0.98150000000000004</v>
-      </c>
-      <c r="M7" s="5">
-        <v>7129</v>
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="M7" s="4">
+        <v>570</v>
       </c>
       <c r="N7" s="4">
-        <v>6.91</v>
+        <v>9.52</v>
       </c>
       <c r="O7" s="4">
-        <v>6.81</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="P7" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q7" s="4">
-        <v>9.66</v>
+        <v>11.1</v>
       </c>
       <c r="R7" s="10">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="S7" s="10">
-        <v>0.66180000000000005</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="T7" s="5">
-        <v>15074282</v>
+        <v>19740515</v>
       </c>
       <c r="U7" s="5">
-        <v>15356929</v>
+        <v>20497102</v>
       </c>
       <c r="V7" s="4">
         <v>27</v>
@@ -1065,67 +1003,67 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="5">
-        <v>99265</v>
+        <v>62425</v>
       </c>
       <c r="C8" s="5">
-        <v>3068855</v>
+        <v>2222421</v>
       </c>
       <c r="D8" s="5">
-        <v>3087655</v>
-      </c>
-      <c r="E8" s="4">
-        <v>-18800</v>
+        <v>2213551</v>
+      </c>
+      <c r="E8" s="5">
+        <v>8870</v>
       </c>
       <c r="F8" s="5">
-        <v>3068855</v>
-      </c>
-      <c r="G8" s="4">
-        <v>-18800</v>
+        <v>2222421</v>
+      </c>
+      <c r="G8" s="5">
+        <v>8870</v>
       </c>
       <c r="H8" s="5">
-        <v>80465</v>
+        <v>71295</v>
       </c>
       <c r="I8" s="5">
-        <v>492445</v>
+        <v>492648</v>
       </c>
       <c r="J8" s="5">
-        <v>625369</v>
+        <v>425114</v>
       </c>
       <c r="K8" s="5">
-        <v>109890</v>
+        <v>71526</v>
       </c>
       <c r="L8" s="10">
-        <v>1.0357000000000001</v>
+        <v>0.98150000000000004</v>
       </c>
       <c r="M8" s="5">
-        <v>7911</v>
+        <v>7129</v>
       </c>
       <c r="N8" s="4">
-        <v>6.12</v>
+        <v>6.91</v>
       </c>
       <c r="O8" s="4">
-        <v>6.3</v>
+        <v>6.81</v>
       </c>
       <c r="P8" s="4">
-        <v>10.17</v>
+        <v>10</v>
       </c>
       <c r="Q8" s="4">
-        <v>13.17</v>
+        <v>9.66</v>
       </c>
       <c r="R8" s="10">
-        <v>0.63</v>
+        <v>0.68</v>
       </c>
       <c r="S8" s="10">
-        <v>0.64639999999999997</v>
+        <v>0.66180000000000005</v>
       </c>
       <c r="T8" s="5">
-        <v>19452226</v>
+        <v>15074282</v>
       </c>
       <c r="U8" s="5">
-        <v>18781392</v>
+        <v>15356929</v>
       </c>
       <c r="V8" s="4">
         <v>27</v>
@@ -1139,280 +1077,334 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5">
+        <v>99265</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3068855</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3087655</v>
+      </c>
+      <c r="E9" s="4">
+        <v>-18800</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3068855</v>
+      </c>
+      <c r="G9" s="4">
+        <v>-18800</v>
+      </c>
+      <c r="H9" s="5">
+        <v>80465</v>
+      </c>
+      <c r="I9" s="5">
+        <v>492445</v>
+      </c>
+      <c r="J9" s="5">
+        <v>625369</v>
+      </c>
+      <c r="K9" s="5">
+        <v>109890</v>
+      </c>
+      <c r="L9" s="10">
+        <v>1.0357000000000001</v>
+      </c>
+      <c r="M9" s="5">
+        <v>7911</v>
+      </c>
+      <c r="N9" s="4">
+        <v>6.12</v>
+      </c>
+      <c r="O9" s="4">
+        <v>6.3</v>
+      </c>
+      <c r="P9" s="4">
+        <v>10.17</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>13.17</v>
+      </c>
+      <c r="R9" s="10">
+        <v>0.63</v>
+      </c>
+      <c r="S9" s="10">
+        <v>0.64639999999999997</v>
+      </c>
+      <c r="T9" s="5">
+        <v>19452226</v>
+      </c>
+      <c r="U9" s="5">
+        <v>18781392</v>
+      </c>
+      <c r="V9" s="4">
+        <v>27</v>
+      </c>
+      <c r="W9" s="4">
+        <v>27</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B10" s="5">
         <v>131883</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C10" s="5">
         <v>4158354</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D10" s="5">
         <v>4108239</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E10" s="5">
         <v>50115</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F10" s="5">
         <v>4158354</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G10" s="5">
         <v>50115</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H10" s="5">
         <v>181998</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I10" s="5">
         <v>1375904</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J10" s="5">
         <v>982528</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K10" s="5">
         <v>128944</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L10" s="10">
         <v>0.97350000000000003</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M10" s="5">
         <v>18199</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N10" s="4">
         <v>7.56</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O10" s="4">
         <v>7.45</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P10" s="4">
         <v>10</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q10" s="4">
         <v>10.98</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R10" s="10">
         <v>0.65</v>
       </c>
-      <c r="S9" s="10">
+      <c r="S10" s="10">
         <v>0.68030000000000002</v>
       </c>
-      <c r="T9" s="5">
+      <c r="T10" s="5">
         <v>30606380</v>
       </c>
-      <c r="U9" s="5">
+      <c r="U10" s="5">
         <v>31437156</v>
       </c>
-      <c r="V9" s="4">
-        <v>27</v>
-      </c>
-      <c r="W9" s="4">
-        <v>27</v>
-      </c>
-      <c r="X9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="V10" s="4">
+        <v>27</v>
+      </c>
+      <c r="W10" s="4">
+        <v>27</v>
+      </c>
+      <c r="X10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B11" s="6">
         <v>530967</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="6">
         <v>16154567</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="6">
         <v>16161550</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E11" s="3">
         <v>-6982.9999999998254</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F11" s="6">
         <v>16154566</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G11" s="3">
         <v>-6984</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H11" s="6">
         <v>523983</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I11" s="6">
         <v>3604036</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J11" s="6">
         <v>3764040</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K11" s="6">
         <v>562897</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L11" s="11">
         <v>0.9849</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M11" s="6">
         <v>7334</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N11" s="3">
         <v>7.21</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O11" s="3">
         <v>6.84</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P11" s="3">
         <v>10.02</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q11" s="3">
         <v>11.26</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="R11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="S11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T10" s="6">
+      <c r="T11" s="6">
         <v>110545002</v>
       </c>
-      <c r="U10" s="6">
+      <c r="U11" s="6">
         <v>112112688</v>
       </c>
-      <c r="V10" s="3">
-        <v>27</v>
-      </c>
-      <c r="W10" s="3">
-        <v>27</v>
-      </c>
-      <c r="X10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="V11" s="3">
+        <v>27</v>
+      </c>
+      <c r="W11" s="3">
+        <v>27</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B12" s="5">
         <v>123410</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <v>3526411</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D12" s="5">
         <v>3503097</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E12" s="5">
         <v>23314</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F12" s="5">
         <v>3526411</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G12" s="5">
         <v>23314</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H12" s="5">
         <v>146724</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I12" s="5">
         <v>589830</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J12" s="5">
         <v>534365</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K12" s="5">
         <v>119367</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L12" s="10">
         <v>1.0699000000000001</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M12" s="5">
         <v>13338</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N12" s="4">
         <v>4.0199999999999996</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O12" s="4">
         <v>4.33</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P12" s="4">
         <v>11</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q12" s="4">
         <v>9.82</v>
       </c>
-      <c r="R11" s="10">
+      <c r="R12" s="10">
         <v>0.8</v>
       </c>
-      <c r="S11" s="10">
+      <c r="S12" s="10">
         <v>0.76439999999999997</v>
       </c>
-      <c r="T11" s="5">
+      <c r="T12" s="5">
         <v>15168410</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U12" s="5">
         <v>14176172</v>
       </c>
-      <c r="V11" s="4">
-        <v>27</v>
-      </c>
-      <c r="W11" s="4">
-        <v>27</v>
-      </c>
-      <c r="X11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="V12" s="4">
+        <v>27</v>
+      </c>
+      <c r="W12" s="4">
+        <v>27</v>
+      </c>
+      <c r="X12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <v>16154567</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B17" s="8">
         <v>16161550</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C17" s="8">
         <v>530000</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
-        <v>16161550</v>
-      </c>
-      <c r="F16" s="9">
-        <v>-6983</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="8">
-        <v>565000</v>
       </c>
       <c r="D17" s="9">
         <v>0</v>
@@ -1432,7 +1424,7 @@
         <v>48</v>
       </c>
       <c r="C18" s="8">
-        <v>600000</v>
+        <v>565000</v>
       </c>
       <c r="D18" s="9">
         <v>0</v>
@@ -1452,7 +1444,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="8">
-        <v>635000</v>
+        <v>600000</v>
       </c>
       <c r="D19" s="9">
         <v>0</v>
@@ -1472,7 +1464,7 @@
         <v>48</v>
       </c>
       <c r="C20" s="8">
-        <v>670000</v>
+        <v>635000</v>
       </c>
       <c r="D20" s="9">
         <v>0</v>
@@ -1492,7 +1484,7 @@
         <v>48</v>
       </c>
       <c r="C21" s="8">
-        <v>705000</v>
+        <v>670000</v>
       </c>
       <c r="D21" s="9">
         <v>0</v>
@@ -1501,6 +1493,26 @@
         <v>16161550</v>
       </c>
       <c r="F21" s="9">
+        <v>-6983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="8">
+        <v>705000</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8">
+        <v>16161550</v>
+      </c>
+      <c r="F22" s="9">
         <v>-6983</v>
       </c>
     </row>

</xml_diff>